<commit_message>
067 radar plot working
</commit_message>
<xml_diff>
--- a/067_types_of_data_professionals/data/types_of_data_professionals.xlsx
+++ b/067_types_of_data_professionals/data/types_of_data_professionals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02-R_Tips\free_r_tips\067_types_of_data_professionals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6230D6FD-3B37-44E7-98B2-5F00C114E787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B9ECF1-2FF8-4F9C-98BE-9D2BA9CDAF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{338C1CBA-6FCF-4D4B-AE63-0785FC4B74CB}"/>
+    <workbookView xWindow="1410" yWindow="1965" windowWidth="16620" windowHeight="10560" xr2:uid="{338C1CBA-6FCF-4D4B-AE63-0785FC4B74CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>